<commit_message>
compare the metrics and plot distribution
</commit_message>
<xml_diff>
--- a/GasEdges.xlsx
+++ b/GasEdges.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21727"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22730"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wany105\OneDrive - Vanderbilt\Research\ShelbyCounty_DataRead\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://vanderbilt365-my.sharepoint.com/personal/yu_wang_1_vanderbilt_edu/Documents/code/Infrastructure-network-simulation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="24" documentId="13_ncr:1_{A60302EB-33CB-47A6-9213-5383CC94C0A7}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{DAF62124-89EB-4DA0-A58A-00AE97EC5B63}"/>
+  <xr:revisionPtr revIDLastSave="38" documentId="13_ncr:1_{A60302EB-33CB-47A6-9213-5383CC94C0A7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{FE1C7EA6-753F-4001-89D8-0F1B2536237F}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="10395" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -366,7 +366,7 @@
   <dimension ref="A1:E19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -393,10 +393,10 @@
         <v>1</v>
       </c>
       <c r="B2" s="1">
+        <v>1</v>
+      </c>
+      <c r="C2" s="1">
         <v>10</v>
-      </c>
-      <c r="C2" s="1">
-        <v>1</v>
       </c>
       <c r="E2" s="1"/>
     </row>
@@ -429,10 +429,10 @@
         <v>4</v>
       </c>
       <c r="B5" s="1">
+        <v>2</v>
+      </c>
+      <c r="C5" s="1">
         <v>6</v>
-      </c>
-      <c r="C5" s="1">
-        <v>2</v>
       </c>
       <c r="E5" s="1"/>
     </row>
@@ -453,10 +453,10 @@
         <v>6</v>
       </c>
       <c r="B7" s="1">
+        <v>8</v>
+      </c>
+      <c r="C7" s="1">
         <v>14</v>
-      </c>
-      <c r="C7" s="1">
-        <v>8</v>
       </c>
       <c r="E7" s="1"/>
     </row>
@@ -489,10 +489,10 @@
         <v>9</v>
       </c>
       <c r="B10" s="1">
+        <v>5</v>
+      </c>
+      <c r="C10" s="1">
         <v>6</v>
-      </c>
-      <c r="C10" s="1">
-        <v>5</v>
       </c>
       <c r="E10" s="1"/>
     </row>
@@ -513,10 +513,10 @@
         <v>11</v>
       </c>
       <c r="B12" s="1">
+        <v>6</v>
+      </c>
+      <c r="C12" s="1">
         <v>11</v>
-      </c>
-      <c r="C12" s="1">
-        <v>6</v>
       </c>
       <c r="E12" s="1"/>
     </row>
@@ -525,10 +525,10 @@
         <v>12</v>
       </c>
       <c r="B13" s="1">
+        <v>3</v>
+      </c>
+      <c r="C13" s="1">
         <v>11</v>
-      </c>
-      <c r="C13" s="1">
-        <v>3</v>
       </c>
       <c r="E13" s="1"/>
     </row>
@@ -561,10 +561,10 @@
         <v>15</v>
       </c>
       <c r="B16" s="1">
+        <v>7</v>
+      </c>
+      <c r="C16" s="1">
         <v>12</v>
-      </c>
-      <c r="C16" s="1">
-        <v>7</v>
       </c>
       <c r="E16" s="1"/>
     </row>

</xml_diff>